<commit_message>
Addition to snake and ladders analysis.
</commit_message>
<xml_diff>
--- a/Homework2/HW2Data/Part2/NullGame/Markov/NullsGameMarkovData.xlsx
+++ b/Homework2/HW2Data/Part2/NullGame/Markov/NullsGameMarkovData.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12756" windowHeight="10956" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="10956" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transition Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="Transition Matrix Probability" sheetId="2" r:id="rId2"/>
+    <sheet name="Probability Distribution Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -87,6 +87,2489 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage chance of finishing game in n-moves</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Probability Distribution Matrix'!$CY$2:$CY$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.7247000000000003E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.05635E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5562799999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.6113099999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1787600000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.110389</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.38142800000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.96876400000000007</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9050199999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0122400000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.9412299999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.3633199999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1608399999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.46746</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.55566</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.6827000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99817099999999992</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.53733699999999995</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26414799999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.119224</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.9642800000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.9148499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.8674800000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.2975199999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.1907999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.11094E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.8257899999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5146499999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.7166699999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.6217800000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.89359E-7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.9427600000000006E-8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.7920600000000005E-9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.4632000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.6131300000000003E-10</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.4420500000000004E-11</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.1925899999999997E-12</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.11004E-12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.63373E-13</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.2940400000000002E-14</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.0744299999999997E-15</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.9336400000000002E-16</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8060099999999999E-17</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.6078000000000003E-18</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.2495299999999997E-19</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.6518699999999997E-20</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.7615500000000001E-21</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.5627599999999994E-22</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.0808600000000004E-23</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.3771099999999995E-24</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.53598E-25</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.6486300000000001E-26</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.7969600000000002E-27</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0420400000000003E-28</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.4188899999999998E-29</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.3750599999999991E-31</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.8848700000000009E-32</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.5057299999999998E-33</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.9796499999999999E-34</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.05826E-35</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.3475600000000006E-37</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.55015E-38</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.1458399999999999E-39</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.8484900000000008E-41</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.8216899999999999E-42</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="291775136"/>
+        <c:axId val="291775920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="291775136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="291775920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="291775920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="291775136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cummulative probability of finishing the game in n-moves</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Percentage Chance of finishing the game</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Probability Distribution Matrix'!$DB$2:$DB$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.01024E-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.53491E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2745599999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0249599999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.3648899999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22101999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.97817799999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.17604</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0310299999999994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.5398</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.7483</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43.442</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58.566099999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>72.089100000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>82.72890000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>90.174900000000008</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>94.852099999999993</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>97.509699999999995</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>98.884700000000009</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>99.5364</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>99.820599999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>99.935299999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>99.978200000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>99.993200000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>99.998000000000005</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>99.999499999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="413578688"/>
+        <c:axId val="413579472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="413578688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of rolls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413579472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="413579472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413578688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>106</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>114</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>106</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>114</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31182,20 +33665,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CW102"/>
+  <dimension ref="A1:DB102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA35" workbookViewId="0">
-      <selection activeCell="CW44" sqref="CW44"/>
+    <sheetView tabSelected="1" topLeftCell="CV68" workbookViewId="0">
+      <selection activeCell="DN102" sqref="DN102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -31499,8 +33982,16 @@
       <c r="CW2">
         <v>0</v>
       </c>
+      <c r="CY2">
+        <f>CV2 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="DB2">
+        <f>CW2 * 100</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -31804,8 +34295,16 @@
       <c r="CW3">
         <v>0</v>
       </c>
+      <c r="CY3">
+        <f t="shared" ref="CY3:CY66" si="0">CV3 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="DB3">
+        <f t="shared" ref="DB3:DB66" si="1">CW3 * 100</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -32109,8 +34608,16 @@
       <c r="CW4">
         <v>0</v>
       </c>
+      <c r="CY4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -32414,8 +34921,16 @@
       <c r="CW5">
         <v>0</v>
       </c>
+      <c r="CY5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -32719,8 +35234,16 @@
       <c r="CW6">
         <v>0</v>
       </c>
+      <c r="CY6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -33024,8 +35547,16 @@
       <c r="CW7">
         <v>0</v>
       </c>
+      <c r="CY7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -33329,8 +35860,16 @@
       <c r="CW8">
         <v>0</v>
       </c>
+      <c r="CY8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -33634,8 +36173,16 @@
       <c r="CW9">
         <v>0</v>
       </c>
+      <c r="CY9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -33939,8 +36486,16 @@
       <c r="CW10">
         <v>0</v>
       </c>
+      <c r="CY10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -34244,8 +36799,16 @@
       <c r="CW11">
         <v>0</v>
       </c>
+      <c r="CY11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -34549,8 +37112,16 @@
       <c r="CW12">
         <v>0</v>
       </c>
+      <c r="CY12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -34854,8 +37425,16 @@
       <c r="CW13">
         <v>0</v>
       </c>
+      <c r="CY13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -35159,8 +37738,16 @@
       <c r="CW14">
         <v>0</v>
       </c>
+      <c r="CY14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -35464,8 +38051,16 @@
       <c r="CW15">
         <v>0</v>
       </c>
+      <c r="CY15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -35769,8 +38364,16 @@
       <c r="CW16">
         <v>0</v>
       </c>
+      <c r="CY16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -36074,8 +38677,16 @@
       <c r="CW17">
         <v>0</v>
       </c>
+      <c r="CY17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -36379,8 +38990,16 @@
       <c r="CW18" s="1">
         <v>1.01024E-11</v>
       </c>
+      <c r="CY18">
+        <f t="shared" si="0"/>
+        <v>5.7247000000000003E-9</v>
+      </c>
+      <c r="DB18">
+        <f t="shared" si="1"/>
+        <v>1.01024E-9</v>
+      </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -36684,8 +39303,16 @@
       <c r="CW19" s="1">
         <v>1.5349099999999999E-8</v>
       </c>
+      <c r="CY19">
+        <f t="shared" si="0"/>
+        <v>3.05635E-6</v>
+      </c>
+      <c r="DB19">
+        <f t="shared" si="1"/>
+        <v>1.53491E-6</v>
+      </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -36989,8 +39616,16 @@
       <c r="CW20" s="1">
         <v>1.27456E-6</v>
       </c>
+      <c r="CY20">
+        <f t="shared" si="0"/>
+        <v>1.5562799999999999E-4</v>
+      </c>
+      <c r="DB20">
+        <f t="shared" si="1"/>
+        <v>1.2745599999999999E-4</v>
+      </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -37294,8 +39929,16 @@
       <c r="CW21" s="1">
         <v>3.0249599999999999E-5</v>
       </c>
+      <c r="CY21">
+        <f t="shared" si="0"/>
+        <v>2.6113099999999999E-3</v>
+      </c>
+      <c r="DB21">
+        <f t="shared" si="1"/>
+        <v>3.0249599999999997E-3</v>
+      </c>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -37599,8 +40242,16 @@
       <c r="CW22">
         <v>3.3648899999999998E-4</v>
       </c>
+      <c r="CY22">
+        <f t="shared" si="0"/>
+        <v>2.1787600000000001E-2</v>
+      </c>
+      <c r="DB22">
+        <f t="shared" si="1"/>
+        <v>3.3648899999999995E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -37904,8 +40555,16 @@
       <c r="CW23">
         <v>2.2101999999999998E-3</v>
       </c>
+      <c r="CY23">
+        <f t="shared" si="0"/>
+        <v>0.110389</v>
+      </c>
+      <c r="DB23">
+        <f t="shared" si="1"/>
+        <v>0.22101999999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -38209,8 +40868,16 @@
       <c r="CW24">
         <v>9.7817800000000003E-3</v>
       </c>
+      <c r="CY24">
+        <f t="shared" si="0"/>
+        <v>0.38142800000000004</v>
+      </c>
+      <c r="DB24">
+        <f t="shared" si="1"/>
+        <v>0.97817799999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -38514,8 +41181,16 @@
       <c r="CW25">
         <v>3.1760400000000001E-2</v>
       </c>
+      <c r="CY25">
+        <f t="shared" si="0"/>
+        <v>0.96876400000000007</v>
+      </c>
+      <c r="DB25">
+        <f t="shared" si="1"/>
+        <v>3.17604</v>
+      </c>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -38819,8 +41494,16 @@
       <c r="CW26">
         <v>8.0310300000000001E-2</v>
       </c>
+      <c r="CY26">
+        <f t="shared" si="0"/>
+        <v>1.9050199999999999</v>
+      </c>
+      <c r="DB26">
+        <f t="shared" si="1"/>
+        <v>8.0310299999999994</v>
+      </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -39124,8 +41807,16 @@
       <c r="CW27">
         <v>0.16539799999999999</v>
       </c>
+      <c r="CY27">
+        <f t="shared" si="0"/>
+        <v>3.0122400000000003</v>
+      </c>
+      <c r="DB27">
+        <f t="shared" si="1"/>
+        <v>16.5398</v>
+      </c>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -39429,8 +42120,16 @@
       <c r="CW28">
         <v>0.28748299999999999</v>
       </c>
+      <c r="CY28">
+        <f t="shared" si="0"/>
+        <v>3.9412299999999996</v>
+      </c>
+      <c r="DB28">
+        <f t="shared" si="1"/>
+        <v>28.7483</v>
+      </c>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -39734,8 +42433,16 @@
       <c r="CW29">
         <v>0.43441999999999997</v>
       </c>
+      <c r="CY29">
+        <f t="shared" si="0"/>
+        <v>4.3633199999999999</v>
+      </c>
+      <c r="DB29">
+        <f t="shared" si="1"/>
+        <v>43.442</v>
+      </c>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -40039,8 +42746,16 @@
       <c r="CW30">
         <v>0.58566099999999999</v>
       </c>
+      <c r="CY30">
+        <f t="shared" si="0"/>
+        <v>4.1608399999999994</v>
+      </c>
+      <c r="DB30">
+        <f t="shared" si="1"/>
+        <v>58.566099999999999</v>
+      </c>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -40344,8 +43059,16 @@
       <c r="CW31">
         <v>0.72089099999999995</v>
       </c>
+      <c r="CY31">
+        <f t="shared" si="0"/>
+        <v>3.46746</v>
+      </c>
+      <c r="DB31">
+        <f t="shared" si="1"/>
+        <v>72.089100000000002</v>
+      </c>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -40649,8 +43372,16 @@
       <c r="CW32">
         <v>0.82728900000000005</v>
       </c>
+      <c r="CY32">
+        <f t="shared" si="0"/>
+        <v>2.55566</v>
+      </c>
+      <c r="DB32">
+        <f t="shared" si="1"/>
+        <v>82.72890000000001</v>
+      </c>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -40954,8 +43685,16 @@
       <c r="CW33">
         <v>0.90174900000000002</v>
       </c>
+      <c r="CY33">
+        <f t="shared" si="0"/>
+        <v>1.6827000000000001</v>
+      </c>
+      <c r="DB33">
+        <f t="shared" si="1"/>
+        <v>90.174900000000008</v>
+      </c>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
@@ -41259,8 +43998,16 @@
       <c r="CW34">
         <v>0.94852099999999995</v>
       </c>
+      <c r="CY34">
+        <f t="shared" si="0"/>
+        <v>0.99817099999999992</v>
+      </c>
+      <c r="DB34">
+        <f t="shared" si="1"/>
+        <v>94.852099999999993</v>
+      </c>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
@@ -41564,8 +44311,16 @@
       <c r="CW35">
         <v>0.97509699999999999</v>
       </c>
+      <c r="CY35">
+        <f t="shared" si="0"/>
+        <v>0.53733699999999995</v>
+      </c>
+      <c r="DB35">
+        <f t="shared" si="1"/>
+        <v>97.509699999999995</v>
+      </c>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -41869,8 +44624,16 @@
       <c r="CW36">
         <v>0.98884700000000003</v>
       </c>
+      <c r="CY36">
+        <f t="shared" si="0"/>
+        <v>0.26414799999999999</v>
+      </c>
+      <c r="DB36">
+        <f t="shared" si="1"/>
+        <v>98.884700000000009</v>
+      </c>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -42174,8 +44937,16 @@
       <c r="CW37">
         <v>0.99536400000000003</v>
       </c>
+      <c r="CY37">
+        <f t="shared" si="0"/>
+        <v>0.119224</v>
+      </c>
+      <c r="DB37">
+        <f t="shared" si="1"/>
+        <v>99.5364</v>
+      </c>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -42479,8 +45250,16 @@
       <c r="CW38">
         <v>0.99820600000000004</v>
       </c>
+      <c r="CY38">
+        <f t="shared" si="0"/>
+        <v>4.9642800000000001E-2</v>
+      </c>
+      <c r="DB38">
+        <f t="shared" si="1"/>
+        <v>99.820599999999999</v>
+      </c>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -42784,8 +45563,16 @@
       <c r="CW39">
         <v>0.99935300000000005</v>
       </c>
+      <c r="CY39">
+        <f t="shared" si="0"/>
+        <v>1.9148499999999999E-2</v>
+      </c>
+      <c r="DB39">
+        <f t="shared" si="1"/>
+        <v>99.935299999999998</v>
+      </c>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
@@ -43089,8 +45876,16 @@
       <c r="CW40">
         <v>0.99978199999999995</v>
       </c>
+      <c r="CY40">
+        <f t="shared" si="0"/>
+        <v>6.8674800000000005E-3</v>
+      </c>
+      <c r="DB40">
+        <f t="shared" si="1"/>
+        <v>99.978200000000001</v>
+      </c>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -43394,8 +46189,16 @@
       <c r="CW41">
         <v>0.99993200000000004</v>
       </c>
+      <c r="CY41">
+        <f t="shared" si="0"/>
+        <v>2.2975199999999999E-3</v>
+      </c>
+      <c r="DB41">
+        <f t="shared" si="1"/>
+        <v>99.993200000000002</v>
+      </c>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -43699,8 +46502,16 @@
       <c r="CW42">
         <v>0.99997999999999998</v>
       </c>
+      <c r="CY42">
+        <f t="shared" si="0"/>
+        <v>7.1907999999999998E-4</v>
+      </c>
+      <c r="DB42">
+        <f t="shared" si="1"/>
+        <v>99.998000000000005</v>
+      </c>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -44004,8 +46815,16 @@
       <c r="CW43">
         <v>0.99999499999999997</v>
       </c>
+      <c r="CY43">
+        <f t="shared" si="0"/>
+        <v>2.11094E-4</v>
+      </c>
+      <c r="DB43">
+        <f t="shared" si="1"/>
+        <v>99.999499999999998</v>
+      </c>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
@@ -44309,8 +47128,16 @@
       <c r="CW44">
         <v>1</v>
       </c>
+      <c r="CY44">
+        <f t="shared" si="0"/>
+        <v>5.8257899999999997E-5</v>
+      </c>
+      <c r="DB44">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
@@ -44614,8 +47441,16 @@
       <c r="CW45">
         <v>1</v>
       </c>
+      <c r="CY45">
+        <f t="shared" si="0"/>
+        <v>1.5146499999999998E-5</v>
+      </c>
+      <c r="DB45">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
@@ -44919,8 +47754,16 @@
       <c r="CW46">
         <v>1</v>
       </c>
+      <c r="CY46">
+        <f t="shared" si="0"/>
+        <v>3.7166699999999999E-6</v>
+      </c>
+      <c r="DB46">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
@@ -45224,8 +48067,16 @@
       <c r="CW47">
         <v>1</v>
       </c>
+      <c r="CY47">
+        <f t="shared" si="0"/>
+        <v>8.6217800000000001E-7</v>
+      </c>
+      <c r="DB47">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -45529,8 +48380,16 @@
       <c r="CW48">
         <v>1</v>
       </c>
+      <c r="CY48">
+        <f t="shared" si="0"/>
+        <v>1.89359E-7</v>
+      </c>
+      <c r="DB48">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -45834,8 +48693,16 @@
       <c r="CW49">
         <v>1</v>
       </c>
+      <c r="CY49">
+        <f t="shared" si="0"/>
+        <v>3.9427600000000006E-8</v>
+      </c>
+      <c r="DB49">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -46139,8 +49006,16 @@
       <c r="CW50">
         <v>1</v>
       </c>
+      <c r="CY50">
+        <f t="shared" si="0"/>
+        <v>7.7920600000000005E-9</v>
+      </c>
+      <c r="DB50">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -46444,8 +49319,16 @@
       <c r="CW51">
         <v>1</v>
       </c>
+      <c r="CY51">
+        <f t="shared" si="0"/>
+        <v>1.4632000000000001E-9</v>
+      </c>
+      <c r="DB51">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -46749,8 +49632,16 @@
       <c r="CW52">
         <v>1</v>
       </c>
+      <c r="CY52">
+        <f t="shared" si="0"/>
+        <v>2.6131300000000003E-10</v>
+      </c>
+      <c r="DB52">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -47054,8 +49945,16 @@
       <c r="CW53">
         <v>1</v>
       </c>
+      <c r="CY53">
+        <f t="shared" si="0"/>
+        <v>4.4420500000000004E-11</v>
+      </c>
+      <c r="DB53">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
@@ -47359,8 +50258,16 @@
       <c r="CW54">
         <v>1</v>
       </c>
+      <c r="CY54">
+        <f t="shared" si="0"/>
+        <v>7.1925899999999997E-12</v>
+      </c>
+      <c r="DB54">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
@@ -47664,8 +50571,16 @@
       <c r="CW55">
         <v>1</v>
       </c>
+      <c r="CY55">
+        <f t="shared" si="0"/>
+        <v>1.11004E-12</v>
+      </c>
+      <c r="DB55">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -47969,8 +50884,16 @@
       <c r="CW56">
         <v>1</v>
       </c>
+      <c r="CY56">
+        <f t="shared" si="0"/>
+        <v>1.63373E-13</v>
+      </c>
+      <c r="DB56">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -48274,8 +51197,16 @@
       <c r="CW57">
         <v>1</v>
       </c>
+      <c r="CY57">
+        <f t="shared" si="0"/>
+        <v>2.2940400000000002E-14</v>
+      </c>
+      <c r="DB57">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
@@ -48579,8 +51510,16 @@
       <c r="CW58">
         <v>1</v>
       </c>
+      <c r="CY58">
+        <f t="shared" si="0"/>
+        <v>3.0744299999999997E-15</v>
+      </c>
+      <c r="DB58">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>0</v>
       </c>
@@ -48884,8 +51823,16 @@
       <c r="CW59">
         <v>1</v>
       </c>
+      <c r="CY59">
+        <f t="shared" si="0"/>
+        <v>3.9336400000000002E-16</v>
+      </c>
+      <c r="DB59">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
@@ -49189,8 +52136,16 @@
       <c r="CW60">
         <v>1</v>
       </c>
+      <c r="CY60">
+        <f t="shared" si="0"/>
+        <v>4.8060099999999999E-17</v>
+      </c>
+      <c r="DB60">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="61" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
@@ -49494,8 +52449,16 @@
       <c r="CW61">
         <v>1</v>
       </c>
+      <c r="CY61">
+        <f t="shared" si="0"/>
+        <v>5.6078000000000003E-18</v>
+      </c>
+      <c r="DB61">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="62" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
@@ -49799,8 +52762,16 @@
       <c r="CW62">
         <v>1</v>
       </c>
+      <c r="CY62">
+        <f t="shared" si="0"/>
+        <v>6.2495299999999997E-19</v>
+      </c>
+      <c r="DB62">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="63" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
@@ -50104,8 +53075,16 @@
       <c r="CW63">
         <v>1</v>
       </c>
+      <c r="CY63">
+        <f t="shared" si="0"/>
+        <v>6.6518699999999997E-20</v>
+      </c>
+      <c r="DB63">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="64" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
@@ -50409,8 +53388,16 @@
       <c r="CW64">
         <v>1</v>
       </c>
+      <c r="CY64">
+        <f t="shared" si="0"/>
+        <v>6.7615500000000001E-21</v>
+      </c>
+      <c r="DB64">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="65" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
@@ -50714,8 +53701,16 @@
       <c r="CW65">
         <v>1</v>
       </c>
+      <c r="CY65">
+        <f t="shared" si="0"/>
+        <v>6.5627599999999994E-22</v>
+      </c>
+      <c r="DB65">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="66" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>0</v>
       </c>
@@ -51019,8 +54014,16 @@
       <c r="CW66">
         <v>1</v>
       </c>
+      <c r="CY66">
+        <f t="shared" si="0"/>
+        <v>6.0808600000000004E-23</v>
+      </c>
+      <c r="DB66">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="67" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>0</v>
       </c>
@@ -51324,8 +54327,16 @@
       <c r="CW67">
         <v>1</v>
       </c>
+      <c r="CY67">
+        <f t="shared" ref="CY67:CY102" si="2">CV67 * 100</f>
+        <v>5.3771099999999995E-24</v>
+      </c>
+      <c r="DB67">
+        <f t="shared" ref="DB67:DB102" si="3">CW67 * 100</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="68" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
@@ -51629,8 +54640,16 @@
       <c r="CW68">
         <v>1</v>
       </c>
+      <c r="CY68">
+        <f t="shared" si="2"/>
+        <v>4.53598E-25</v>
+      </c>
+      <c r="DB68">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="69" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
@@ -51934,8 +54953,16 @@
       <c r="CW69">
         <v>1</v>
       </c>
+      <c r="CY69">
+        <f t="shared" si="2"/>
+        <v>3.6486300000000001E-26</v>
+      </c>
+      <c r="DB69">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="70" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>0</v>
       </c>
@@ -52239,8 +55266,16 @@
       <c r="CW70">
         <v>1</v>
       </c>
+      <c r="CY70">
+        <f t="shared" si="2"/>
+        <v>2.7969600000000002E-27</v>
+      </c>
+      <c r="DB70">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="71" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
@@ -52544,8 +55579,16 @@
       <c r="CW71">
         <v>1</v>
       </c>
+      <c r="CY71">
+        <f t="shared" si="2"/>
+        <v>2.0420400000000003E-28</v>
+      </c>
+      <c r="DB71">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="72" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
@@ -52849,8 +55892,16 @@
       <c r="CW72">
         <v>1</v>
       </c>
+      <c r="CY72">
+        <f t="shared" si="2"/>
+        <v>1.4188899999999998E-29</v>
+      </c>
+      <c r="DB72">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="73" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
@@ -53154,8 +56205,16 @@
       <c r="CW73">
         <v>1</v>
       </c>
+      <c r="CY73">
+        <f t="shared" si="2"/>
+        <v>9.3750599999999991E-31</v>
+      </c>
+      <c r="DB73">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="74" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
@@ -53459,8 +56518,16 @@
       <c r="CW74">
         <v>1</v>
       </c>
+      <c r="CY74">
+        <f t="shared" si="2"/>
+        <v>5.8848700000000009E-32</v>
+      </c>
+      <c r="DB74">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="75" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
@@ -53764,8 +56831,16 @@
       <c r="CW75">
         <v>1</v>
       </c>
+      <c r="CY75">
+        <f t="shared" si="2"/>
+        <v>3.5057299999999998E-33</v>
+      </c>
+      <c r="DB75">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="76" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>0</v>
       </c>
@@ -54069,8 +57144,16 @@
       <c r="CW76">
         <v>1</v>
       </c>
+      <c r="CY76">
+        <f t="shared" si="2"/>
+        <v>1.9796499999999999E-34</v>
+      </c>
+      <c r="DB76">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="77" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -54374,8 +57457,16 @@
       <c r="CW77">
         <v>1</v>
       </c>
+      <c r="CY77">
+        <f t="shared" si="2"/>
+        <v>1.05826E-35</v>
+      </c>
+      <c r="DB77">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="78" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>0</v>
       </c>
@@ -54679,8 +57770,16 @@
       <c r="CW78">
         <v>1</v>
       </c>
+      <c r="CY78">
+        <f t="shared" si="2"/>
+        <v>5.3475600000000006E-37</v>
+      </c>
+      <c r="DB78">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="79" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
@@ -54984,8 +58083,16 @@
       <c r="CW79">
         <v>1</v>
       </c>
+      <c r="CY79">
+        <f t="shared" si="2"/>
+        <v>2.55015E-38</v>
+      </c>
+      <c r="DB79">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="80" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>0</v>
       </c>
@@ -55289,8 +58396,16 @@
       <c r="CW80">
         <v>1</v>
       </c>
+      <c r="CY80">
+        <f t="shared" si="2"/>
+        <v>1.1458399999999999E-39</v>
+      </c>
+      <c r="DB80">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="81" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
@@ -55594,8 +58709,16 @@
       <c r="CW81">
         <v>1</v>
       </c>
+      <c r="CY81">
+        <f t="shared" si="2"/>
+        <v>4.8484900000000008E-41</v>
+      </c>
+      <c r="DB81">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="82" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
@@ -55899,8 +59022,16 @@
       <c r="CW82">
         <v>1</v>
       </c>
+      <c r="CY82">
+        <f t="shared" si="2"/>
+        <v>1.8216899999999999E-42</v>
+      </c>
+      <c r="DB82">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="83" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -56204,8 +59335,16 @@
       <c r="CW83">
         <v>1</v>
       </c>
+      <c r="CY83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB83">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="84" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -56509,8 +59648,16 @@
       <c r="CW84">
         <v>1</v>
       </c>
+      <c r="CY84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB84">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="85" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
@@ -56814,8 +59961,16 @@
       <c r="CW85">
         <v>1</v>
       </c>
+      <c r="CY85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB85">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="86" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
@@ -57119,8 +60274,16 @@
       <c r="CW86">
         <v>1</v>
       </c>
+      <c r="CY86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB86">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="87" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
@@ -57424,8 +60587,16 @@
       <c r="CW87">
         <v>1</v>
       </c>
+      <c r="CY87">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB87">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="88" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
@@ -57729,8 +60900,16 @@
       <c r="CW88">
         <v>1</v>
       </c>
+      <c r="CY88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB88">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="89" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
@@ -58034,8 +61213,16 @@
       <c r="CW89">
         <v>1</v>
       </c>
+      <c r="CY89">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB89">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="90" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
@@ -58339,8 +61526,16 @@
       <c r="CW90">
         <v>1</v>
       </c>
+      <c r="CY90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB90">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="91" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0</v>
       </c>
@@ -58644,8 +61839,16 @@
       <c r="CW91">
         <v>1</v>
       </c>
+      <c r="CY91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB91">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="92" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
@@ -58949,8 +62152,16 @@
       <c r="CW92">
         <v>1</v>
       </c>
+      <c r="CY92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB92">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="93" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
@@ -59254,8 +62465,16 @@
       <c r="CW93">
         <v>1</v>
       </c>
+      <c r="CY93">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB93">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="94" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>0</v>
       </c>
@@ -59559,8 +62778,16 @@
       <c r="CW94">
         <v>1</v>
       </c>
+      <c r="CY94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB94">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="95" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
@@ -59864,8 +63091,16 @@
       <c r="CW95">
         <v>1</v>
       </c>
+      <c r="CY95">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB95">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="96" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>0</v>
       </c>
@@ -60169,8 +63404,16 @@
       <c r="CW96">
         <v>1</v>
       </c>
+      <c r="CY96">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB96">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="97" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>0</v>
       </c>
@@ -60474,8 +63717,16 @@
       <c r="CW97">
         <v>1</v>
       </c>
+      <c r="CY97">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB97">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="98" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
@@ -60779,8 +64030,16 @@
       <c r="CW98">
         <v>1</v>
       </c>
+      <c r="CY98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB98">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="99" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0</v>
       </c>
@@ -61084,8 +64343,16 @@
       <c r="CW99">
         <v>1</v>
       </c>
+      <c r="CY99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB99">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="100" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>0</v>
       </c>
@@ -61389,8 +64656,16 @@
       <c r="CW100">
         <v>1</v>
       </c>
+      <c r="CY100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB100">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="101" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>0</v>
       </c>
@@ -61694,8 +64969,16 @@
       <c r="CW101">
         <v>1</v>
       </c>
+      <c r="CY101">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB101">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="102" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -61998,9 +65281,18 @@
       </c>
       <c r="CW102">
         <v>1</v>
+      </c>
+      <c r="CY102">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="DB102">
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Snakes and ladders data files
</commit_message>
<xml_diff>
--- a/Homework2/HW2Data/Part2/NullGame/Markov/NullsGameMarkovData.xlsx
+++ b/Homework2/HW2Data/Part2/NullGame/Markov/NullsGameMarkovData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RCP\UCF\IDS6938\MyRepository\IDS6938-SimulationTechniques\Homework2\HW2Data\Part2\NullGame\Markov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RCP\UCF\Modeling_and_Simulation\IDS6938_Spring2017\MyRepository\IDS6938-SimulationTechniques\Homework2\HW2Data\Part2\NullGame\Markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="10956" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="10950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transition Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="Probability Distribution Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -130,12 +130,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Null Game Markov</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Percentage chance of finishing game in n-moves</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -511,6 +518,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1066-4957-81F5-371497762681}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -520,6 +532,20 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
         <c:smooth val="0"/>
         <c:axId val="291775136"/>
         <c:axId val="291775920"/>
@@ -531,6 +557,64 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of rolls</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -594,8 +678,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of work complete %</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -685,7 +827,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -725,12 +867,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cummulative probability of finishing the game in n-moves</a:t>
+              <a:t>Null Game Markov Cummulative probability of finishing the game in n-moves</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1109,6 +1250,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8E0-4FD9-84EC-7E241115E874}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1168,7 +1314,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1280,12 +1425,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percentage</a:t>
+                  <a:t>Percentage %</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1356,37 +1500,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2511,20 +2624,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>106</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>107</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>114</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>318135</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2541,20 +2660,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>106</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>114</xdr:col>
+      <xdr:colOff>316230</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>186690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>114</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>122</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>186690</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2648,6 +2773,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2683,6 +2825,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2841,19 +3000,19 @@
       <selection activeCell="A2" sqref="A2:CX103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3158,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3463,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3768,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4073,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4378,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4683,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4988,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -5293,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -5598,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -5903,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -6208,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -6513,7 +6672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -6818,7 +6977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -7123,7 +7282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -7428,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -7733,7 +7892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -8038,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -8343,7 +8502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -8648,7 +8807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -8953,7 +9112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -9258,7 +9417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -9563,7 +9722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -9868,7 +10027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -10173,7 +10332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -10478,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -10783,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -11088,7 +11247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -11393,7 +11552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -11698,7 +11857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -12003,7 +12162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -12308,7 +12467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -12613,7 +12772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -12918,7 +13077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -13223,7 +13382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -13528,7 +13687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -13833,7 +13992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -14138,7 +14297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -14443,7 +14602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -14748,7 +14907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -15053,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -15358,7 +15517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -15663,7 +15822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -15968,7 +16127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -16273,7 +16432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -16578,7 +16737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -16883,7 +17042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -17188,7 +17347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -17493,7 +17652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -17798,7 +17957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -18103,7 +18262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -18408,7 +18567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -18713,7 +18872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -19018,7 +19177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -19323,7 +19482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -19628,7 +19787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -19933,7 +20092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -20238,7 +20397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -20543,7 +20702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -20848,7 +21007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -21153,7 +21312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -21458,7 +21617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -21763,7 +21922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -22068,7 +22227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -22373,7 +22532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -22678,7 +22837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -22983,7 +23142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -23288,7 +23447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -23593,7 +23752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -23898,7 +24057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -24203,7 +24362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -24508,7 +24667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -24813,7 +24972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -25118,7 +25277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -25423,7 +25582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -25728,7 +25887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -26033,7 +26192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -26338,7 +26497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -26643,7 +26802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -26948,7 +27107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -27253,7 +27412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -27558,7 +27717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -27863,7 +28022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -28168,7 +28327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -28473,7 +28632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -28778,7 +28937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -29083,7 +29242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -29388,7 +29547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -29693,7 +29852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -29998,7 +30157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -30303,7 +30462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -30608,7 +30767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -30913,7 +31072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -31218,7 +31377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -31523,7 +31682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -31828,7 +31987,7 @@
         <v>0.16666700000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -32133,7 +32292,7 @@
         <v>0.33333299999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -32438,7 +32597,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -32743,7 +32902,7 @@
         <v>0.66666700000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -33048,7 +33207,7 @@
         <v>0.83333299999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -33353,7 +33512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -33667,18 +33826,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CV68" workbookViewId="0">
-      <selection activeCell="DN102" sqref="DN102"/>
+    <sheetView tabSelected="1" topLeftCell="DB68" workbookViewId="0">
+      <selection activeCell="DK94" sqref="DK94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -33991,7 +34150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -34304,7 +34463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -34617,7 +34776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -34930,7 +35089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -35243,7 +35402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -35556,7 +35715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -35869,7 +36028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -36182,7 +36341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -36495,7 +36654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -36808,7 +36967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -37121,7 +37280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -37434,7 +37593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -37747,7 +37906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -38060,7 +38219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -38373,7 +38532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -38686,7 +38845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -38999,7 +39158,7 @@
         <v>1.01024E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -39312,7 +39471,7 @@
         <v>1.53491E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -39625,7 +39784,7 @@
         <v>1.2745599999999999E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -39938,7 +40097,7 @@
         <v>3.0249599999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -40251,7 +40410,7 @@
         <v>3.3648899999999995E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -40564,7 +40723,7 @@
         <v>0.22101999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -40877,7 +41036,7 @@
         <v>0.97817799999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -41190,7 +41349,7 @@
         <v>3.17604</v>
       </c>
     </row>
-    <row r="26" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -41503,7 +41662,7 @@
         <v>8.0310299999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -41816,7 +41975,7 @@
         <v>16.5398</v>
       </c>
     </row>
-    <row r="28" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -42129,7 +42288,7 @@
         <v>28.7483</v>
       </c>
     </row>
-    <row r="29" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -42442,7 +42601,7 @@
         <v>43.442</v>
       </c>
     </row>
-    <row r="30" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -42755,7 +42914,7 @@
         <v>58.566099999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -43068,7 +43227,7 @@
         <v>72.089100000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -43381,7 +43540,7 @@
         <v>82.72890000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -43694,7 +43853,7 @@
         <v>90.174900000000008</v>
       </c>
     </row>
-    <row r="34" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -44007,7 +44166,7 @@
         <v>94.852099999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -44320,7 +44479,7 @@
         <v>97.509699999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -44633,7 +44792,7 @@
         <v>98.884700000000009</v>
       </c>
     </row>
-    <row r="37" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -44946,7 +45105,7 @@
         <v>99.5364</v>
       </c>
     </row>
-    <row r="38" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -45259,7 +45418,7 @@
         <v>99.820599999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -45572,7 +45731,7 @@
         <v>99.935299999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -45885,7 +46044,7 @@
         <v>99.978200000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -46198,7 +46357,7 @@
         <v>99.993200000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -46511,7 +46670,7 @@
         <v>99.998000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -46824,7 +46983,7 @@
         <v>99.999499999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -47137,7 +47296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -47450,7 +47609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -47763,7 +47922,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -48076,7 +48235,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -48389,7 +48548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -48702,7 +48861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -49015,7 +49174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -49328,7 +49487,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -49641,7 +49800,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -49954,7 +50113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -50267,7 +50426,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -50580,7 +50739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -50893,7 +51052,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -51206,7 +51365,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -51519,7 +51678,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -51832,7 +51991,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -52145,7 +52304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -52458,7 +52617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -52771,7 +52930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -53084,7 +53243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -53397,7 +53556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -53710,7 +53869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -54023,7 +54182,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -54336,7 +54495,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -54649,7 +54808,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -54962,7 +55121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -55275,7 +55434,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -55588,7 +55747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -55901,7 +56060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -56214,7 +56373,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -56527,7 +56686,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -56840,7 +56999,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -57153,7 +57312,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -57466,7 +57625,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -57779,7 +57938,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -58092,7 +58251,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -58405,7 +58564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -58718,7 +58877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -59031,7 +59190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -59344,7 +59503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -59657,7 +59816,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -59970,7 +60129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -60283,7 +60442,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -60596,7 +60755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -60909,7 +61068,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -61222,7 +61381,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -61535,7 +61694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -61848,7 +62007,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -62161,7 +62320,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -62474,7 +62633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -62787,7 +62946,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -63100,7 +63259,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -63413,7 +63572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -63726,7 +63885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -64039,7 +64198,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -64352,7 +64511,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -64665,7 +64824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -64978,7 +65137,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>

</xml_diff>